<commit_message>
Updated VBA script and screenshots
</commit_message>
<xml_diff>
--- a/Screenshots_Multiple_year_stock_data.xlsx
+++ b/Screenshots_Multiple_year_stock_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijet\Desktop\DataViz\Homework\VBA-challenge\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF1E33A-C471-4E15-998D-79AA89A3CB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67EE023-908E-4EAA-8488-03D9BA325CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="2015" sheetId="2" r:id="rId2"/>
     <sheet name="2014" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,148 +87,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FF6A846-613F-4AAD-B439-E7609EF7701A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="13049250" cy="6896100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEF43DE-3F1B-484B-8773-CEFABD35E24C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="13068300" cy="6915150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28498F91-D898-459B-AF7D-C70E66845B50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFBFB5E3-AC05-4480-AC76-1AC9496486D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -253,6 +121,138 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="13011150" cy="6915150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73815F17-7193-4D2E-8E96-94A0C9D867D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13011150" cy="6934200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8AF89A-2B68-4205-88EC-87D8CA58816A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13049250" cy="6934200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -540,7 +540,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>